<commit_message>
[FIX] view excel in gl_webkit and query item from DB
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_revenue_ledger.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_revenue_ledger.xlsx
@@ -314,16 +314,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -335,11 +339,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -433,8 +433,8 @@
   </sheetPr>
   <dimension ref="A1:BB12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AP8" activeCellId="0" sqref="AP8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,79 +446,88 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="8" style="1" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="1" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="15.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="19" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="40" min="24" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="42" min="41" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="44" min="44" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="45" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2"/>
+      <c r="A1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="12" s="10" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="12" s="10" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
[IMP] Adjust Revenue Ledger
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_revenue_ledger.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_revenue_ledger.xlsx
@@ -221,9 +221,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="165" formatCode="#,###.00"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -309,7 +310,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,6 +323,14 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -334,7 +343,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,261 +442,386 @@
   </sheetPr>
   <dimension ref="A1:BB12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP8" activeCellId="0" sqref="AP8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="1" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="13" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="19" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="40" min="24" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="42" min="41" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="44" min="44" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="45" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="2" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="21.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="4" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="4" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="23.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="21.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="24.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="23.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="4" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="4" width="22.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="4" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="1" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="1" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="24.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="23.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="54" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5"/>
+      <c r="L1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AR1" s="2"/>
+    </row>
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="L2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AR2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="7"/>
+      <c r="L3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AR3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="7"/>
+      <c r="L4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AR4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="D5" s="7"/>
+      <c r="L5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AR5" s="2"/>
+    </row>
+    <row r="6" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="7"/>
+      <c r="L6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AR6" s="2"/>
+    </row>
+    <row r="7" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="D7" s="7"/>
+      <c r="L7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AR7" s="2"/>
+    </row>
+    <row r="8" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="D8" s="8"/>
+      <c r="L8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AR8" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="B9" s="7"/>
+      <c r="L9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AR9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="12" s="10" customFormat="true" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="B10" s="8"/>
+      <c r="L10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AR10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AR11" s="2"/>
+    </row>
+    <row r="12" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="8" t="s">
+      <c r="N12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="8" t="s">
+      <c r="O12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="8" t="s">
+      <c r="P12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Q12" s="8" t="s">
+      <c r="Q12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R12" s="8" t="s">
+      <c r="R12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="T12" s="8" t="s">
+      <c r="T12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="U12" s="8" t="s">
+      <c r="U12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="V12" s="8" t="s">
+      <c r="V12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="W12" s="8" t="s">
+      <c r="W12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="X12" s="8" t="s">
+      <c r="X12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="Y12" s="8" t="s">
+      <c r="Y12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="Z12" s="8" t="s">
+      <c r="Z12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="AA12" s="8" t="s">
+      <c r="AA12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="AB12" s="8" t="s">
+      <c r="AB12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AC12" s="8" t="s">
+      <c r="AC12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AD12" s="8" t="s">
+      <c r="AD12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AE12" s="8" t="s">
+      <c r="AE12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AF12" s="8" t="s">
+      <c r="AF12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AG12" s="8" t="s">
+      <c r="AG12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="AH12" s="8" t="s">
+      <c r="AH12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="AI12" s="8" t="s">
+      <c r="AI12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="AJ12" s="8" t="s">
+      <c r="AJ12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AK12" s="8" t="s">
+      <c r="AK12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="AL12" s="8" t="s">
+      <c r="AL12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="AM12" s="8" t="s">
+      <c r="AM12" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AN12" s="8" t="s">
+      <c r="AN12" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AO12" s="8" t="s">
+      <c r="AO12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="AP12" s="8" t="s">
+      <c r="AP12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AQ12" s="8" t="s">
+      <c r="AQ12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="AR12" s="8" t="s">
+      <c r="AR12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="AS12" s="8" t="s">
+      <c r="AS12" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="AT12" s="8" t="s">
+      <c r="AT12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AU12" s="8" t="s">
+      <c r="AU12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AV12" s="8" t="s">
+      <c r="AV12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="AW12" s="8" t="s">
+      <c r="AW12" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AX12" s="8" t="s">
+      <c r="AX12" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="AY12" s="8" t="s">
+      <c r="AY12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AZ12" s="8" t="s">
+      <c r="AZ12" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="BA12" s="8" t="s">
+      <c r="BA12" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="BB12" s="9"/>
+      <c r="BB12" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>